<commit_message>
Add liquid viscosity and density calculate tests
</commit_message>
<xml_diff>
--- a/BatchTest.xlsx
+++ b/BatchTest.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal_master/VESIcal/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/Published Papers/2021_VESIcal/__TheCode/VESIcal_master/VESIcal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5477A0-DE68-D142-A4C3-FAF9EB33AF47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A90FD77-DC01-284C-8F15-BC9663A57AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22680" yWindow="7000" windowWidth="28040" windowHeight="17440" xr2:uid="{D5D8394A-7272-CB4F-A3ED-C86444CC2A22}"/>
+    <workbookView xWindow="10360" yWindow="4160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D5D8394A-7272-CB4F-A3ED-C86444CC2A22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="giordano_test" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Label</t>
   </si>
@@ -79,6 +81,18 @@
   </si>
   <si>
     <t>test_samp</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>F2O</t>
+  </si>
+  <si>
+    <t>giordano_spreadsheet_default_comp</t>
+  </si>
+  <si>
+    <t>test_w_F</t>
   </si>
 </sst>
 </file>
@@ -432,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFDF7A7-BC3F-EC42-B16C-14580102E372}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,4 +543,219 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7889A671-981D-F04B-A273-6F211412B587}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>47.95</v>
+      </c>
+      <c r="C2">
+        <v>1.67</v>
+      </c>
+      <c r="D2">
+        <v>17.32</v>
+      </c>
+      <c r="E2">
+        <v>10.24</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <v>5.76</v>
+      </c>
+      <c r="H2">
+        <v>10.93</v>
+      </c>
+      <c r="I2">
+        <v>3.45</v>
+      </c>
+      <c r="J2">
+        <v>1.99</v>
+      </c>
+      <c r="K2">
+        <v>0.51</v>
+      </c>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>0.1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>62.4</v>
+      </c>
+      <c r="C3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D3">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="E3">
+        <v>0.03</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>3.22</v>
+      </c>
+      <c r="H3">
+        <v>9.08</v>
+      </c>
+      <c r="I3">
+        <v>3.52</v>
+      </c>
+      <c r="J3">
+        <v>0.93</v>
+      </c>
+      <c r="K3">
+        <v>0.12</v>
+      </c>
+      <c r="L3">
+        <v>0.02</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>47.95</v>
+      </c>
+      <c r="C4">
+        <v>1.67</v>
+      </c>
+      <c r="D4">
+        <v>17.32</v>
+      </c>
+      <c r="E4">
+        <v>10.24</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4">
+        <v>5.76</v>
+      </c>
+      <c r="H4">
+        <v>10.93</v>
+      </c>
+      <c r="I4">
+        <v>3.45</v>
+      </c>
+      <c r="J4">
+        <v>1.99</v>
+      </c>
+      <c r="K4">
+        <v>0.51</v>
+      </c>
+      <c r="L4">
+        <v>0.1</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>0.1</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>